<commit_message>
created: starters import preview
</commit_message>
<xml_diff>
--- a/web/template_en.xlsx
+++ b/web/template_en.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gaming\Documents\uteg\web\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="21075" windowHeight="12585"/>
   </bookViews>
@@ -94,7 +99,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -107,10 +112,10 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -125,20 +130,23 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F2"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Firstname" dataDxfId="6"/>
-    <tableColumn id="2" name="Lastname" dataDxfId="5"/>
-    <tableColumn id="3" name="Birth year" dataDxfId="4"/>
-    <tableColumn id="4" name="Sex" dataDxfId="3"/>
-    <tableColumn id="5" name="Category" dataDxfId="2"/>
-    <tableColumn id="6" name="Club" dataDxfId="1"/>
+    <tableColumn id="1" name="Firstname" dataDxfId="5"/>
+    <tableColumn id="2" name="Lastname" dataDxfId="4"/>
+    <tableColumn id="3" name="Birth year" dataDxfId="3"/>
+    <tableColumn id="4" name="Sex" dataDxfId="2"/>
+    <tableColumn id="5" name="Category" dataDxfId="1"/>
+    <tableColumn id="6" name="Club" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -187,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,10 +443,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
@@ -524,7 +532,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -536,7 +544,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
grade entering nearly finished logo in ranking report validation modal in judging
</commit_message>
<xml_diff>
--- a/web/template_en.xlsx
+++ b/web/template_en.xlsx
@@ -1,27 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gaming\Documents\uteg\web\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="21075" windowHeight="12585"/>
+    <workbookView windowWidth="28695" windowHeight="13635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+  <si>
+    <t>STV-ID</t>
+  </si>
   <si>
     <t>Firstname</t>
   </si>
@@ -40,44 +38,372 @@
   <si>
     <t>Club</t>
   </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Mathias</t>
-  </si>
-  <si>
-    <t>Scherer</t>
-  </si>
-  <si>
-    <t>STV Wettingen</t>
-  </si>
-  <si>
-    <t>K5</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -85,68 +411,330 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="50">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Standard" xfId="42"/>
+    <cellStyle name="20% - Accent1" xfId="43" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="46" builtinId="17"/>
+    <cellStyle name="Comma" xfId="47" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="48" builtinId="23"/>
+    <cellStyle name="Percent" xfId="49" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:G2" totalsRowShown="0">
+  <autoFilter ref="B1:G2"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Firstname" dataDxfId="5"/>
-    <tableColumn id="2" name="Lastname" dataDxfId="4"/>
-    <tableColumn id="3" name="Birth year" dataDxfId="3"/>
-    <tableColumn id="4" name="Sex" dataDxfId="2"/>
-    <tableColumn id="5" name="Category" dataDxfId="1"/>
-    <tableColumn id="6" name="Club" dataDxfId="0"/>
+    <tableColumn id="1" name="Firstname"/>
+    <tableColumn id="2" name="Lastname"/>
+    <tableColumn id="3" name="Birth year"/>
+    <tableColumn id="4" name="Sex"/>
+    <tableColumn id="5" name="Category"/>
+    <tableColumn id="6" name="Club"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -157,7 +745,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="5B6469"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -195,7 +783,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +818,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,25 +1026,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.4285714285714" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.4285714285714" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8571428571429" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.8571428571429" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1428571428571" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,77 +1065,72 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1994</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="2" spans="4:4">
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0"/>
+  <sheetProtection selectLockedCells="1" insertRows="0" deleteRows="0" sort="0"/>
   <dataValidations count="6">
-    <dataValidation type="textLength" operator="equal" showInputMessage="1" showErrorMessage="1" promptTitle="Birth year" prompt="Enter the starter's birth year" sqref="C2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Choose starter's category" sqref="F2">
+      <formula1>"K1,K2,K3,K4,K5,K6,K7,KD/H,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Sex" prompt="Choose the starter's sex" sqref="E2">
+      <formula1>"Male,Female"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Firstname" prompt="Enter starter's firstname" sqref="B2">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Lastname" prompt="Enter starter's lastname" sqref="C2">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Club" prompt="Enter starter's club name" sqref="G2">
+      <formula1>5</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showInputMessage="1" showErrorMessage="1" promptTitle="Birth year" prompt="Enter the starter's birth year" sqref="D2">
       <formula1>4</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Sex" prompt="Choose the starter's sex" sqref="D2">
-      <formula1>"Male,Female"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Firstname" prompt="Enter starter's firstname" sqref="A2">
-      <formula1>2</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Lastname" prompt="Enter starter's lastname" sqref="B2">
-      <formula1>2</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Choose starter's category" sqref="E2">
-      <formula1>"K1,K2,K3,K4,K5,K6,K7,KD/H,"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Club" prompt="Enter starter's club name" sqref="F2">
-      <formula1>5</formula1>
-    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes a shitload of bugs and adds a lot of new features done with a new version which I found on my old laptop .... injects the complete vender because of some customizations / I know never do this but I was young :)
</commit_message>
<xml_diff>
--- a/web/template_en.xlsx
+++ b/web/template_en.xlsx
@@ -1,27 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gaming\Documents\uteg\web\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="21075" windowHeight="12585"/>
+    <workbookView windowWidth="28695" windowHeight="13635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+  <si>
+    <t>STV-ID</t>
+  </si>
   <si>
     <t>Firstname</t>
   </si>
@@ -40,44 +38,372 @@
   <si>
     <t>Club</t>
   </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Mathias</t>
-  </si>
-  <si>
-    <t>Scherer</t>
-  </si>
-  <si>
-    <t>STV Wettingen</t>
-  </si>
-  <si>
-    <t>K5</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -85,68 +411,330 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="50">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Standard" xfId="42"/>
+    <cellStyle name="20% - Accent1" xfId="43" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="46" builtinId="17"/>
+    <cellStyle name="Comma" xfId="47" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="48" builtinId="23"/>
+    <cellStyle name="Percent" xfId="49" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:G2" totalsRowShown="0">
+  <autoFilter ref="B1:G2"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Firstname" dataDxfId="5"/>
-    <tableColumn id="2" name="Lastname" dataDxfId="4"/>
-    <tableColumn id="3" name="Birth year" dataDxfId="3"/>
-    <tableColumn id="4" name="Sex" dataDxfId="2"/>
-    <tableColumn id="5" name="Category" dataDxfId="1"/>
-    <tableColumn id="6" name="Club" dataDxfId="0"/>
+    <tableColumn id="1" name="Firstname"/>
+    <tableColumn id="2" name="Lastname"/>
+    <tableColumn id="3" name="Birth year"/>
+    <tableColumn id="4" name="Sex"/>
+    <tableColumn id="5" name="Category"/>
+    <tableColumn id="6" name="Club"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -157,7 +745,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="5B6469"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -195,7 +783,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +818,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,25 +1026,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.4285714285714" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.4285714285714" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8571428571429" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.8571428571429" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1428571428571" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,77 +1065,72 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1994</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="2" spans="4:4">
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0"/>
+  <sheetProtection selectLockedCells="1" insertRows="0" deleteRows="0" sort="0"/>
   <dataValidations count="6">
-    <dataValidation type="textLength" operator="equal" showInputMessage="1" showErrorMessage="1" promptTitle="Birth year" prompt="Enter the starter's birth year" sqref="C2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Choose starter's category" sqref="F2">
+      <formula1>"K1,K2,K3,K4,K5,K6,K7,KD/H,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Sex" prompt="Choose the starter's sex" sqref="E2">
+      <formula1>"Male,Female"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Firstname" prompt="Enter starter's firstname" sqref="B2">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Lastname" prompt="Enter starter's lastname" sqref="C2">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Club" prompt="Enter starter's club name" sqref="G2">
+      <formula1>5</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showInputMessage="1" showErrorMessage="1" promptTitle="Birth year" prompt="Enter the starter's birth year" sqref="D2">
       <formula1>4</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Sex" prompt="Choose the starter's sex" sqref="D2">
-      <formula1>"Male,Female"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Firstname" prompt="Enter starter's firstname" sqref="A2">
-      <formula1>2</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Lastname" prompt="Enter starter's lastname" sqref="B2">
-      <formula1>2</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Choose starter's category" sqref="E2">
-      <formula1>"K1,K2,K3,K4,K5,K6,K7,KD/H,"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Club" prompt="Enter starter's club name" sqref="F2">
-      <formula1>5</formula1>
-    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>